<commit_message>
Update test file, more meaningful examples
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/complex_1.xlsx
+++ b/tests/integration_test_files/complex_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863A23D5-D3B1-E449-AC0C-EA5DBE394E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54E4D88D-B114-5F46-9019-F50E320984F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="4260" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="4560" yWindow="3320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="349">
   <si>
     <t>Epoch</t>
   </si>
@@ -1117,6 +1117,12 @@
   </si>
   <si>
     <t>Clinical trials,Washington,'',Washngton DC,12345,USA</t>
+  </si>
+  <si>
+    <t>Study Treatment Administration</t>
+  </si>
+  <si>
+    <t>Insulin Infusion</t>
   </si>
 </sst>
 </file>
@@ -1348,10 +1354,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2929,7 +2935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -3048,32 +3054,32 @@
       <c r="A3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -3204,16 +3210,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3390,7 +3396,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4046,11 +4052,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DCBC64-AD78-403D-83E2-03FD5CA19DE2}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4092,7 +4098,7 @@
         <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>124</v>
+        <v>348</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>8</v>
@@ -4362,7 +4368,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4408,7 +4414,7 @@
         <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>124</v>
+        <v>347</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Further objectives and endpoints fix
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/complex_1.xlsx
+++ b/tests/integration_test_files/complex_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B5FD0B-A2D8-A54A-9F09-6022B00AE20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E15AE3-B8FD-1F48-A237-439690C4A824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38220" yWindow="5160" windowWidth="29040" windowHeight="15840" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="48860" yWindow="9900" windowWidth="42200" windowHeight="15840" firstSheet="2" activeTab="11" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="353">
   <si>
     <t>Epoch</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>endpointDescription</t>
-  </si>
-  <si>
-    <t>endpointPurposeDescription</t>
   </si>
   <si>
     <t>endpointLevel</t>
@@ -1027,14 +1024,6 @@
     <t>TL: TreatmentPhase</t>
   </si>
   <si>
-    <t>To demonstrate that 3 mg LY900018 is non-inferior to 1 mg IMG for the proportion of patients achieving
-treatment success from insulin-induced hypoglycemia using a non-inferiority margin of 10%</t>
-  </si>
-  <si>
-    <t>The proportion of patients achieving treatment success defined as either an increase in PG to &gt;70 mg/dL or an increase of &gt;20 mg/dL from nadir within 30 minutes after administration of glucagon. The nadir is defined
-as the minimum PG value at the time of or within 10 minutes following glucagon administration.</t>
-  </si>
-  <si>
     <t>To compare the safety and tolerability of 3 mg LY900018 with 1 mg IMG</t>
   </si>
   <si>
@@ -1123,6 +1112,27 @@
   </si>
   <si>
     <t>CROSS1</t>
+  </si>
+  <si>
+    <t>objectiveLabel</t>
+  </si>
+  <si>
+    <t>objectiveText</t>
+  </si>
+  <si>
+    <t>endpointLabel</t>
+  </si>
+  <si>
+    <t>endpointText</t>
+  </si>
+  <si>
+    <t>endpointPurpose</t>
+  </si>
+  <si>
+    <t>The proportion of patients achieving treatment success defined as either an increase in PG to &gt;70 mg/dL or an increase of &gt;20 mg/dL from nadir within 30 minutes after administration of glucagon. The nadir is defined as the minimum PG value at the time of or within 10 minutes following glucagon administration.</t>
+  </si>
+  <si>
+    <t>To demonstrate that 3 mg LY900018 is non-inferior to 1 mg IMG for the proportion of patients achieving treatment success from insulin-induced hypoglycemia using a non-inferiority margin of 10%</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1288,9 +1298,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1348,10 +1355,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1690,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1707,10 +1714,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1722,7 +1729,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1767,10 +1774,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1779,10 +1786,10 @@
     </row>
     <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1791,7 +1798,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="11"/>
       <c r="E8" s="1"/>
@@ -1801,10 +1808,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1813,10 +1820,10 @@
     </row>
     <row r="10" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1825,10 +1832,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1837,10 +1844,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1849,7 +1856,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>16</v>
@@ -1861,10 +1868,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1962,7 +1969,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>34</v>
@@ -1976,7 +1983,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -1990,7 +1997,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -2004,7 +2011,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
@@ -2018,7 +2025,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -2129,261 +2136,354 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="59.5" customWidth="1"/>
-    <col min="6" max="7" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="59.5" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="G1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="F2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="K3" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>319</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="F4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>322</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>325</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2410,81 +2510,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E2" t="s">
         <v>328</v>
       </c>
-      <c r="C2" t="s">
-        <v>332</v>
-      </c>
-      <c r="D2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>331</v>
-      </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
         <v>109</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
         <v>110</v>
       </c>
-      <c r="C5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>111</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
         <v>112</v>
-      </c>
-      <c r="F5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2513,82 +2613,82 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>125</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="24" t="s">
-        <v>250</v>
+      <c r="E5" s="23" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2617,147 +2717,147 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>134</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2784,104 +2884,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>149</v>
-      </c>
       <c r="D1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>134</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>295</v>
+      <c r="E2" s="33" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>302</v>
+        <v>150</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>301</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>294</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>296</v>
+        <v>299</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>303</v>
+        <v>151</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>302</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>294</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>296</v>
+        <v>300</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D5" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>297</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>299</v>
+      <c r="D6" s="33" t="s">
+        <v>298</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2906,18 +3006,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2967,39 +3067,39 @@
         <v>30</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E3" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>285</v>
-      </c>
-      <c r="D2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" t="s">
-        <v>283</v>
-      </c>
-      <c r="F2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="D3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>287</v>
-      </c>
       <c r="F3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -3024,25 +3124,25 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="B1" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
+        <v>162</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
@@ -3057,137 +3157,137 @@
       <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
+      <c r="B4" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
+      <c r="B5" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
+      <c r="B6" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="B7" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="B8" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
+        <v>114</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>334</v>
-      </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+        <v>115</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B14" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
-        <v>305</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3204,16 +3304,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3239,53 +3339,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="E2" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
         <v>304</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>306</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>335</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="33" t="s">
+        <v>332</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
-        <v>305</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>307</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>335</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3313,13 +3413,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>167</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3327,43 +3427,43 @@
         <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>333</v>
+        <v>170</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3371,10 +3471,10 @@
         <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3404,10 +3504,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>117</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>0</v>
@@ -3415,33 +3515,33 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="L1" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
       <c r="P1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>2</v>
@@ -3462,10 +3562,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>8</v>
@@ -3531,111 +3631,111 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F6" s="35" t="s">
         <v>336</v>
       </c>
-      <c r="G6" s="35" t="s">
-        <v>336</v>
-      </c>
-      <c r="H6" s="35" t="s">
-        <v>336</v>
+      <c r="F6" s="34" t="s">
+        <v>333</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>333</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>333</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="K6" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="L6" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="L6" s="35" t="s">
-        <v>293</v>
-      </c>
       <c r="M6" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="N6" s="35" t="s">
-        <v>338</v>
-      </c>
-      <c r="O6" s="35" t="s">
-        <v>337</v>
+        <v>333</v>
+      </c>
+      <c r="N6" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="O6" s="34" t="s">
+        <v>334</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="G7" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="M7" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="37"/>
+        <v>144</v>
+      </c>
+      <c r="D8" s="36"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="L8" s="36" t="s">
-        <v>216</v>
+      <c r="L8" s="35" t="s">
+        <v>215</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -3646,18 +3746,18 @@
         <v>7</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>217</v>
+      <c r="B10" s="22" t="s">
+        <v>216</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
@@ -3678,8 +3778,8 @@
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>253</v>
+      <c r="B11" s="22" t="s">
+        <v>252</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="2"/>
@@ -3695,39 +3795,39 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>208</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="23" t="s">
+      <c r="J13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
         <v>220</v>
-      </c>
-      <c r="C13" t="s">
-        <v>209</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="23" t="s">
-        <v>221</v>
       </c>
       <c r="C14"/>
       <c r="D14" s="1" t="s">
@@ -3735,66 +3835,66 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" s="23" t="s">
+      <c r="C16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>204</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="C17" t="s">
-        <v>205</v>
-      </c>
       <c r="D17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="23" t="s">
-        <v>226</v>
+      <c r="B18" s="22" t="s">
+        <v>225</v>
       </c>
       <c r="C18"/>
       <c r="G18" s="1" t="s">
@@ -3814,8 +3914,8 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="23" t="s">
-        <v>227</v>
+      <c r="B19" s="22" t="s">
+        <v>226</v>
       </c>
       <c r="C19"/>
       <c r="D19" s="1" t="s">
@@ -3850,22 +3950,22 @@
       </c>
     </row>
     <row r="20" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" t="s">
+        <v>313</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B21" s="30" t="s">
         <v>230</v>
-      </c>
-      <c r="C20" t="s">
-        <v>314</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="31" t="s">
-        <v>231</v>
       </c>
       <c r="C21"/>
       <c r="H21" s="1" t="s">
@@ -3876,11 +3976,11 @@
       </c>
     </row>
     <row r="22" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="31" t="s">
-        <v>232</v>
+      <c r="B22" s="30" t="s">
+        <v>231</v>
       </c>
       <c r="C22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>5</v>
@@ -3890,22 +3990,22 @@
       </c>
     </row>
     <row r="23" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="22" t="s">
         <v>235</v>
-      </c>
-      <c r="C23" t="s">
-        <v>206</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="23" t="s">
-        <v>236</v>
       </c>
       <c r="C24"/>
       <c r="D24" s="1" t="s">
@@ -3916,116 +4016,116 @@
       </c>
     </row>
     <row r="25" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="22" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B26" s="23" t="s">
+      <c r="D26" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="23" t="s">
+      <c r="D27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B30" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B31" s="23" t="s">
+      <c r="D31" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B32" s="23" t="s">
+      <c r="D32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B33" s="23" t="s">
+      <c r="P33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="P33" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B34" s="23" t="s">
+    </row>
+    <row r="35" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" s="22" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B35" s="23" t="s">
+      <c r="E35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="B36" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="23" t="s">
+      <c r="G36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="B37" s="22" t="s">
         <v>245</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="B37" s="23" t="s">
-        <v>246</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>5</v>
@@ -4063,10 +4163,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>0</v>
@@ -4074,33 +4174,33 @@
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
@@ -4108,10 +4208,10 @@
       <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
@@ -4119,10 +4219,10 @@
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
@@ -4130,42 +4230,42 @@
       <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="H6" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>309</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>313</v>
-      </c>
-      <c r="H6" s="30" t="s">
+      <c r="I6" s="29" t="s">
         <v>311</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+        <v>144</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
@@ -4175,179 +4275,179 @@
         <v>7</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="23" t="s">
-        <v>223</v>
+      <c r="B10" s="22" t="s">
+        <v>222</v>
       </c>
       <c r="C10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+        <v>203</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B11" s="23" t="s">
-        <v>225</v>
+      <c r="B11" s="22" t="s">
+        <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>229</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
+        <v>228</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="C12"/>
-      <c r="D12" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="23" t="s">
+      <c r="C13"/>
+      <c r="D13" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="C13"/>
-      <c r="D13" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="23" t="s">
-        <v>235</v>
-      </c>
       <c r="C14" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+        <v>205</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="B15" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B16" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
+      <c r="B16" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="2:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="2:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="D17" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="2:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
+      <c r="D18" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
       <c r="I18" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B20" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+    </row>
+    <row r="21" spans="2:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B21" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="D20" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-    </row>
-    <row r="21" spans="2:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="B21" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="39"/>
+      <c r="D21" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4375,50 +4475,50 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
@@ -4426,12 +4526,12 @@
       <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
@@ -4439,12 +4539,12 @@
       <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
@@ -4452,71 +4552,71 @@
       <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="J6" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="K6" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="L6" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="N6" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="O6" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="P6" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q6" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="R6" s="29" t="s">
         <v>315</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>269</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>281</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>273</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>274</v>
-      </c>
-      <c r="L6" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="M6" s="30" t="s">
-        <v>276</v>
-      </c>
-      <c r="N6" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="O6" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="P6" s="30" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q6" s="30" t="s">
-        <v>280</v>
-      </c>
-      <c r="R6" s="30" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
+        <v>144</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
@@ -4526,15 +4626,15 @@
         <v>7</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="23" t="s">
-        <v>223</v>
+      <c r="B10" s="22" t="s">
+        <v>222</v>
       </c>
       <c r="C10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -4554,8 +4654,8 @@
       </c>
     </row>
     <row r="11" spans="1:18" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B11" s="23" t="s">
-        <v>230</v>
+      <c r="B11" s="22" t="s">
+        <v>229</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="7"/>
@@ -4576,11 +4676,11 @@
       <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:18" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
-        <v>235</v>
+      <c r="B12" s="22" t="s">
+        <v>234</v>
       </c>
       <c r="C12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>5</v>
@@ -4610,8 +4710,8 @@
       </c>
     </row>
     <row r="13" spans="1:18" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="23" t="s">
-        <v>237</v>
+      <c r="B13" s="22" t="s">
+        <v>236</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>5</v>
@@ -4641,8 +4741,8 @@
       </c>
     </row>
     <row r="14" spans="1:18" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" s="23" t="s">
-        <v>242</v>
+      <c r="B14" s="22" t="s">
+        <v>241</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>5</v>
@@ -4686,8 +4786,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
-        <v>243</v>
+      <c r="B15" s="22" t="s">
+        <v>242</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>5</v>
@@ -4732,25 +4832,25 @@
     </row>
     <row r="16" spans="1:18" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B17" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="B17" s="23" t="s">
-        <v>248</v>
-      </c>
       <c r="D17" s="1" t="s">
         <v>5</v>
       </c>
@@ -4768,11 +4868,11 @@
       </c>
     </row>
     <row r="18" spans="2:18" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="31" t="s">
-        <v>228</v>
+      <c r="B18" s="30" t="s">
+        <v>227</v>
       </c>
       <c r="C18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R18" t="s">
         <v>5</v>
@@ -4804,394 +4904,394 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="C1" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C14" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C16" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="C3" s="26" t="b">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="C5" s="26" t="b">
+      <c r="D23" s="25" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="C25" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="D7" s="26"/>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
-        <v>226</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>256</v>
-      </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
-        <v>227</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>257</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="C14" s="26" t="b">
+      <c r="D25" s="25" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="C27" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="26" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="C16" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="C17" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="C23" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="C25" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="26" t="s">
+      <c r="D27" s="25" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="C27" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B29" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B31" s="25" t="s">
         <v>243</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B32" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B33" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B34" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>247</v>
-      </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
     </row>
     <row r="35" spans="1:4" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
+        <v>247</v>
+      </c>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
+      <c r="A36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweak to example file
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/complex_1.xlsx
+++ b/tests/integration_test_files/complex_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E53D2CC-12F6-7649-AC01-701A76E0C69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52094C1-38B7-164A-A674-6259D0AF08E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24780" yWindow="500" windowWidth="67920" windowHeight="26240" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="46440" yWindow="500" windowWidth="46260" windowHeight="26240" firstSheet="1" activeTab="15" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -1610,7 +1610,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1698,12 +1698,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF444444"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1829,10 +1823,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2165,7 +2159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2432,7 +2426,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="71.5" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
@@ -3535,7 +3529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -3890,10 +3884,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3958,29 +3952,29 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>82</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B3" t="s">
         <v>83</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C3" t="s">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D3" t="s">
         <v>84</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E3" t="s">
         <v>85</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G3" t="s">
         <v>52</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H3" t="s">
         <v>86</v>
       </c>
     </row>
@@ -4511,7 +4505,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+      <selection activeCell="A13" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4547,32 +4541,32 @@
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
@@ -4703,16 +4697,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4723,8 +4717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7FA707-26D8-0546-9A99-D418F7F4E088}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4885,8 +4879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="E43" sqref="E43"/>

</xml_diff>

<commit_message>
Tweak test data and dont add titles if blank
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/complex_1.xlsx
+++ b/tests/integration_test_files/complex_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52094C1-38B7-164A-A674-6259D0AF08E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D308C14-7E31-ED45-922E-65F04EC1800D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46440" yWindow="500" windowWidth="46260" windowHeight="26240" firstSheet="1" activeTab="15" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="46440" yWindow="500" windowWidth="46260" windowHeight="26240" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="508">
   <si>
     <t>Screening</t>
   </si>
@@ -288,9 +288,6 @@
     <t>protocolStatus</t>
   </si>
   <si>
-    <t>Something Public</t>
-  </si>
-  <si>
     <t>Somethign Clever</t>
   </si>
   <si>
@@ -525,13 +522,7 @@
     <t>Data Generated Within Study</t>
   </si>
   <si>
-    <t>Cross Over 1</t>
-  </si>
-  <si>
     <t>Test of a cross over study</t>
-  </si>
-  <si>
-    <t>Cross Over</t>
   </si>
   <si>
     <t>Period 1</t>
@@ -1604,6 +1595,12 @@
   </si>
   <si>
     <t>Discretion</t>
+  </si>
+  <si>
+    <t>A Phase 3 Study of Nasal Glucagon (LY900018) Compared to Intramuscular Glucagon for Treatment of Insulin-induced Hypoglycemia in Japanese Patients with Diabetes Mellitus</t>
+  </si>
+  <si>
+    <t>A Study of Nasal Glucagon (LY900018) in Japanese Participants With Diabetes Mellitus</t>
   </si>
 </sst>
 </file>
@@ -2159,14 +2156,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57.1640625" customWidth="1"/>
     <col min="3" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="16" style="5" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" style="5" customWidth="1"/>
@@ -2176,22 +2173,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>150</v>
+      <c r="B2" s="9" t="s">
+        <v>506</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2251,7 +2248,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2260,7 +2257,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="9"/>
       <c r="E8" s="1"/>
@@ -2268,24 +2265,24 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>152</v>
+      <c r="B9" s="9" t="s">
+        <v>507</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2296,9 +2293,7 @@
       <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="B11" s="7"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -2309,7 +2304,7 @@
         <v>68</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2333,7 +2328,7 @@
         <v>70</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2435,134 +2430,134 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B4" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B5" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B6" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B7" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B8" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B9" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -2591,32 +2586,32 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
       <c r="F1" s="18" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -2625,13 +2620,13 @@
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -2639,18 +2634,18 @@
         <v>1</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -2659,13 +2654,13 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -2673,18 +2668,18 @@
         <v>1</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -2693,13 +2688,13 @@
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -2707,13 +2702,13 @@
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -2722,13 +2717,13 @@
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -2737,13 +2732,13 @@
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -2752,13 +2747,13 @@
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -2767,13 +2762,13 @@
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -2782,13 +2777,13 @@
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -2797,13 +2792,13 @@
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -2811,18 +2806,18 @@
         <v>1</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -2831,13 +2826,13 @@
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -2845,18 +2840,18 @@
         <v>1</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2864,18 +2859,18 @@
         <v>1</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -2884,13 +2879,13 @@
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -2899,13 +2894,13 @@
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -2914,13 +2909,13 @@
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -2929,13 +2924,13 @@
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -2944,13 +2939,13 @@
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -2958,18 +2953,18 @@
         <v>1</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -2978,13 +2973,13 @@
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
@@ -2992,18 +2987,18 @@
         <v>1</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
@@ -3012,13 +3007,13 @@
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
@@ -3026,18 +3021,18 @@
         <v>1</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
@@ -3046,13 +3041,13 @@
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
@@ -3061,13 +3056,13 @@
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
@@ -3076,13 +3071,13 @@
     </row>
     <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
@@ -3091,13 +3086,13 @@
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
@@ -3106,13 +3101,13 @@
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
@@ -3121,13 +3116,13 @@
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="23"/>
@@ -3136,13 +3131,13 @@
     </row>
     <row r="35" spans="1:7" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -3194,61 +3189,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>28</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>307</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -3256,58 +3251,58 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E2" t="s">
         <v>311</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>313</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>314</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="I2" t="s">
         <v>315</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>316</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>317</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>318</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>319</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>320</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>321</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>322</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>323</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>324</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" s="33" t="s">
         <v>325</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>326</v>
-      </c>
-      <c r="R2" t="s">
-        <v>327</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -3315,58 +3310,58 @@
         <v>46</v>
       </c>
       <c r="B3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>312</v>
+      </c>
+      <c r="G3" t="s">
+        <v>313</v>
+      </c>
+      <c r="H3" t="s">
         <v>329</v>
       </c>
-      <c r="C3" t="s">
+      <c r="I3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J3" t="s">
         <v>330</v>
       </c>
-      <c r="D3" t="s">
-        <v>313</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="K3" t="s">
         <v>331</v>
       </c>
-      <c r="F3" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="G3" t="s">
-        <v>316</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>332</v>
       </c>
-      <c r="I3" t="s">
-        <v>318</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
+        <v>319</v>
+      </c>
+      <c r="N3" t="s">
+        <v>320</v>
+      </c>
+      <c r="O3" t="s">
+        <v>321</v>
+      </c>
+      <c r="P3" t="s">
         <v>333</v>
       </c>
-      <c r="K3" t="s">
-        <v>334</v>
-      </c>
-      <c r="L3" t="s">
-        <v>335</v>
-      </c>
-      <c r="M3" t="s">
-        <v>322</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>323</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>324</v>
       </c>
-      <c r="P3" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>326</v>
-      </c>
-      <c r="R3" t="s">
-        <v>327</v>
-      </c>
       <c r="S3" s="33" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3391,13 +3386,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>28</v>
@@ -3408,10 +3403,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>29</v>
@@ -3422,10 +3417,10 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>30</v>
@@ -3457,25 +3452,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>32</v>
@@ -3483,10 +3478,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -3500,24 +3495,24 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G3" t="s">
         <v>342</v>
-      </c>
-      <c r="B3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G3" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -3555,10 +3550,10 @@
         <v>34</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>35</v>
@@ -3570,13 +3565,13 @@
         <v>36</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>37</v>
@@ -3588,7 +3583,7 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>38</v>
@@ -3598,7 +3593,7 @@
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>39</v>
@@ -3610,7 +3605,7 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>40</v>
@@ -3620,7 +3615,7 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>41</v>
@@ -3628,11 +3623,11 @@
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>40</v>
@@ -3642,7 +3637,7 @@
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
@@ -3651,11 +3646,11 @@
     </row>
     <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>40</v>
@@ -3665,7 +3660,7 @@
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
@@ -3886,8 +3881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+    <sheetView topLeftCell="D1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3931,16 +3926,16 @@
         <v>59</v>
       </c>
       <c r="B2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E2" t="s">
         <v>267</v>
-      </c>
-      <c r="C2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" t="s">
-        <v>270</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
@@ -3949,24 +3944,24 @@
         <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
         <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
       </c>
       <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
-      </c>
-      <c r="E3" t="s">
-        <v>85</v>
       </c>
       <c r="F3" t="s">
         <v>46</v>
@@ -3975,7 +3970,7 @@
         <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4001,87 +3996,87 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -4113,144 +4108,144 @@
         <v>42</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -4280,101 +4275,101 @@
         <v>42</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="D1" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E2" s="28" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="D6" s="28" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -4389,7 +4384,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4426,39 +4421,39 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" t="s">
         <v>239</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="D3" t="s">
-        <v>242</v>
-      </c>
       <c r="E3" s="26" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -4481,18 +4476,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
         <v>79</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -4517,10 +4512,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -4528,10 +4523,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -4551,7 +4546,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
@@ -4562,7 +4557,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
@@ -4573,7 +4568,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
@@ -4584,7 +4579,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
@@ -4595,7 +4590,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
@@ -4603,10 +4598,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
@@ -4614,10 +4609,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
@@ -4625,19 +4620,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>15</v>
@@ -4645,42 +4640,42 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -4732,53 +4727,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>146</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4806,13 +4801,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4820,43 +4815,43 @@
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -4864,10 +4859,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -4896,60 +4891,60 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="C1" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>
@@ -4957,13 +4952,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="C3" s="10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -4973,139 +4968,139 @@
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="10" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>365</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="10" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="10" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>15</v>
@@ -5115,46 +5110,46 @@
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="G8" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G8" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="M8" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -5165,15 +5160,15 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -5192,7 +5187,7 @@
     </row>
     <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="2"/>
@@ -5209,10 +5204,10 @@
     </row>
     <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
@@ -5223,10 +5218,10 @@
     </row>
     <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>1</v>
@@ -5240,7 +5235,7 @@
     </row>
     <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C14"/>
       <c r="D14" s="1" t="s">
@@ -5249,7 +5244,7 @@
     </row>
     <row r="15" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="1" t="s">
@@ -5282,10 +5277,10 @@
     </row>
     <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -5296,10 +5291,10 @@
     </row>
     <row r="17" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -5307,7 +5302,7 @@
     </row>
     <row r="18" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="20" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C18"/>
       <c r="G18" s="1" t="s">
@@ -5328,7 +5323,7 @@
     </row>
     <row r="19" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C19"/>
       <c r="D19" s="1" t="s">
@@ -5364,10 +5359,10 @@
     </row>
     <row r="20" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="25" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C20" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>1</v>
@@ -5378,7 +5373,7 @@
     </row>
     <row r="21" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C21"/>
       <c r="H21" s="1" t="s">
@@ -5390,10 +5385,10 @@
     </row>
     <row r="22" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="25" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>1</v>
@@ -5404,10 +5399,10 @@
     </row>
     <row r="23" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>1</v>
@@ -5418,7 +5413,7 @@
     </row>
     <row r="24" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C24"/>
       <c r="D24" s="1" t="s">
@@ -5430,12 +5425,12 @@
     </row>
     <row r="25" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>1</v>
@@ -5443,7 +5438,7 @@
     </row>
     <row r="27" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1</v>
@@ -5454,7 +5449,7 @@
     </row>
     <row r="28" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>1</v>
@@ -5465,7 +5460,7 @@
     </row>
     <row r="29" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>1</v>
@@ -5482,7 +5477,7 @@
     </row>
     <row r="30" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" s="20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>1</v>
@@ -5490,7 +5485,7 @@
     </row>
     <row r="31" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="20" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>1</v>
@@ -5498,7 +5493,7 @@
     </row>
     <row r="32" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="20" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>1</v>
@@ -5506,7 +5501,7 @@
     </row>
     <row r="33" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" s="20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>1</v>
@@ -5514,12 +5509,12 @@
     </row>
     <row r="34" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="20" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
@@ -5527,7 +5522,7 @@
     </row>
     <row r="36" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="20" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>1</v>
@@ -5538,7 +5533,7 @@
     </row>
     <row r="37" spans="2:16" ht="34" x14ac:dyDescent="0.2">
       <c r="B37" s="20" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>1</v>
@@ -5573,39 +5568,39 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G1" t="s">
         <v>422</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>423</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>424</v>
-      </c>
-      <c r="G1" t="s">
-        <v>425</v>
-      </c>
-      <c r="H1" t="s">
-        <v>426</v>
-      </c>
-      <c r="I1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>
@@ -5619,13 +5614,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -5641,68 +5636,68 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="10" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D5" t="s">
+        <v>420</v>
+      </c>
+      <c r="E5" t="s">
+        <v>421</v>
+      </c>
+      <c r="F5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G5" t="s">
         <v>423</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>424</v>
       </c>
-      <c r="F5" t="s">
-        <v>425</v>
-      </c>
-      <c r="G5" t="s">
-        <v>426</v>
-      </c>
-      <c r="H5" t="s">
-        <v>427</v>
-      </c>
       <c r="I5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="10" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="10" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5713,15 +5708,15 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -5731,10 +5726,10 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>1</v>
@@ -5746,7 +5741,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="30" t="s">
@@ -5761,7 +5756,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="30" t="s">
@@ -5776,10 +5771,10 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>1</v>
@@ -5791,7 +5786,7 @@
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="30" t="s">
@@ -5805,7 +5800,7 @@
     </row>
     <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>1</v>
@@ -5817,7 +5812,7 @@
     </row>
     <row r="17" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>1</v>
@@ -5829,7 +5824,7 @@
     </row>
     <row r="18" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>1</v>
@@ -5844,7 +5839,7 @@
     </row>
     <row r="19" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
@@ -5854,7 +5849,7 @@
     </row>
     <row r="20" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>1</v>
@@ -5867,7 +5862,7 @@
     </row>
     <row r="21" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" s="20" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>1</v>
@@ -5907,66 +5902,66 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G1" t="s">
         <v>393</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>394</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>395</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>396</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>397</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>398</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>399</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>400</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>401</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>402</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>403</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>404</v>
-      </c>
-      <c r="P1" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>406</v>
-      </c>
-      <c r="R1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>
@@ -5988,13 +5983,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -6018,108 +6013,108 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="J4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="K4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="L4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="M4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="O4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="P4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="Q4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="R4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="10" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D5" t="s">
+        <v>391</v>
+      </c>
+      <c r="E5" t="s">
+        <v>392</v>
+      </c>
+      <c r="F5" t="s">
+        <v>393</v>
+      </c>
+      <c r="G5" t="s">
         <v>394</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>395</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>396</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>397</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>398</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>399</v>
       </c>
-      <c r="J5" t="s">
+      <c r="M5" t="s">
         <v>400</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>401</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>402</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>403</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>404</v>
       </c>
-      <c r="O5" t="s">
-        <v>405</v>
-      </c>
-      <c r="P5" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>407</v>
-      </c>
       <c r="R5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="10" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D6" s="23"/>
     </row>
@@ -6127,7 +6122,7 @@
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="10" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D7" s="23"/>
     </row>
@@ -6135,7 +6130,7 @@
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="10" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D8" s="23"/>
     </row>
@@ -6147,15 +6142,15 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="Q10" s="5" t="s">
         <v>1</v>
@@ -6164,7 +6159,7 @@
     </row>
     <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C11"/>
       <c r="E11" s="5" t="s">
@@ -6174,10 +6169,10 @@
     </row>
     <row r="12" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>1</v>
@@ -6201,7 +6196,7 @@
     </row>
     <row r="13" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>1</v>
@@ -6225,7 +6220,7 @@
     </row>
     <row r="14" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -6270,7 +6265,7 @@
     </row>
     <row r="15" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>1</v>
@@ -6315,7 +6310,7 @@
     </row>
     <row r="16" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -6343,7 +6338,7 @@
     </row>
     <row r="17" spans="2:18" ht="34" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -6373,10 +6368,10 @@
     </row>
     <row r="18" spans="2:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R18" t="s">
         <v>1</v>
@@ -6408,834 +6403,834 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D1" s="35" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="35" t="s">
+        <v>363</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>364</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>365</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>366</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>367</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>368</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>369</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E3" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G4" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H4" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G5" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E6" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F6" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G6" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G7" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E8" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F8" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G8" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>379</v>
+      </c>
+      <c r="B9" t="s">
         <v>382</v>
-      </c>
-      <c r="B9" t="s">
-        <v>385</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E9" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F9" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G9" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H9" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B10" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E10" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F10" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G10" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H10" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E11" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F11" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G11" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B12" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E12" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F12" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G12" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="H12" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E13" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F13" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G13" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H13" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>386</v>
+      </c>
+      <c r="B14" t="s">
         <v>389</v>
-      </c>
-      <c r="B14" t="s">
-        <v>392</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E14" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F14" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H14" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B15" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E15" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F15" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G15" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H15" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E16" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F16" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G16" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B17" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E17" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F17" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G17" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H17" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B18" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E18" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F18" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G18" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B19" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E19" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F19" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G19" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="H19" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B20" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E20" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F20" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G20" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H20" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B21" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C21"/>
       <c r="D21" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E21" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F21" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G21" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H21" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B22" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E22" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G22" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H22" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B23" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C23"/>
       <c r="D23" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E23" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F23" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G23" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H23" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B24" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C24"/>
       <c r="D24" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E24" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F24" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G24" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="H24" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B25" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E25" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F25" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G25" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H25" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B26" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C26"/>
       <c r="D26" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E26" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F26" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G26" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H26" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B27" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C27"/>
       <c r="D27" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E27" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F27" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G27" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H27" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B28" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C28"/>
       <c r="D28" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E28" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F28" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G28" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="H28" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E29" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F29" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H29" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B30" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C30"/>
       <c r="D30" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E30" t="s">
+        <v>419</v>
+      </c>
+      <c r="F30" t="s">
         <v>422</v>
       </c>
-      <c r="F30" t="s">
-        <v>425</v>
-      </c>
       <c r="G30" s="23" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H30" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B31" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C31"/>
       <c r="D31" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E31" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F31" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G31" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H31" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B32" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C32"/>
       <c r="D32" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E32" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F32" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G32" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H32" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E33" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F33" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G33" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H33"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B34" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C34"/>
       <c r="D34" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E34" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="F34" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G34" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H34" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E35" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F35" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G35" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H35" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further test data tweaks
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/complex_1.xlsx
+++ b/tests/integration_test_files/complex_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D308C14-7E31-ED45-922E-65F04EC1800D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52C5CC6-B780-954F-92D8-64DF6359637F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="46440" yWindow="500" windowWidth="46260" windowHeight="26240" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="505">
   <si>
     <t>Screening</t>
   </si>
@@ -267,9 +267,6 @@
     <t>studyRationale</t>
   </si>
   <si>
-    <t>SIMPLE</t>
-  </si>
-  <si>
     <t>briefTitle</t>
   </si>
   <si>
@@ -286,9 +283,6 @@
   </si>
   <si>
     <t>protocolStatus</t>
-  </si>
-  <si>
-    <t>Somethign Clever</t>
   </si>
   <si>
     <t>draft</t>
@@ -914,9 +908,6 @@
   </si>
   <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>CROSS1</t>
   </si>
   <si>
     <t>objectiveLabel</t>
@@ -2157,7 +2148,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2173,10 +2164,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>279</v>
+        <v>230</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2188,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2235,9 +2226,7 @@
       <c r="A6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="B6" s="7"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -2248,7 +2237,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2257,7 +2246,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="9"/>
       <c r="E8" s="1"/>
@@ -2267,10 +2256,10 @@
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2279,10 +2268,10 @@
     </row>
     <row r="10" spans="1:8" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2291,7 +2280,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="7"/>
       <c r="E11" s="1"/>
@@ -2301,11 +2290,9 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>71</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B12" s="7"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -2313,7 +2300,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>8</v>
@@ -2325,10 +2312,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2430,134 +2417,134 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B3" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B4" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B6" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B7" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B8" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B9" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -2586,32 +2573,32 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
       <c r="F1" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
@@ -2620,13 +2607,13 @@
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -2634,18 +2621,18 @@
         <v>1</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
@@ -2654,13 +2641,13 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -2668,18 +2655,18 @@
         <v>1</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -2688,13 +2675,13 @@
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -2702,13 +2689,13 @@
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -2717,13 +2704,13 @@
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -2732,13 +2719,13 @@
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -2747,13 +2734,13 @@
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -2762,13 +2749,13 @@
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -2777,13 +2764,13 @@
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -2792,13 +2779,13 @@
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -2806,18 +2793,18 @@
         <v>1</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -2826,13 +2813,13 @@
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -2840,18 +2827,18 @@
         <v>1</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2859,18 +2846,18 @@
         <v>1</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -2879,13 +2866,13 @@
     </row>
     <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -2894,13 +2881,13 @@
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -2909,13 +2896,13 @@
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -2924,13 +2911,13 @@
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -2939,13 +2926,13 @@
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -2953,18 +2940,18 @@
         <v>1</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -2973,13 +2960,13 @@
     </row>
     <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
@@ -2987,18 +2974,18 @@
         <v>1</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="23"/>
@@ -3007,13 +2994,13 @@
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
@@ -3021,18 +3008,18 @@
         <v>1</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
@@ -3041,13 +3028,13 @@
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
@@ -3056,13 +3043,13 @@
     </row>
     <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
@@ -3071,13 +3058,13 @@
     </row>
     <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
@@ -3086,13 +3073,13 @@
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
@@ -3101,13 +3088,13 @@
     </row>
     <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
@@ -3116,13 +3103,13 @@
     </row>
     <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="23"/>
@@ -3131,13 +3118,13 @@
     </row>
     <row r="35" spans="1:7" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -3189,61 +3176,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>28</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>26</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -3251,58 +3238,58 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E2" t="s">
         <v>308</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" s="32" t="s">
         <v>309</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>310</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>311</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="I2" t="s">
         <v>312</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>313</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>314</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>315</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>316</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>317</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>318</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>319</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>320</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>321</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" s="33" t="s">
         <v>322</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>323</v>
-      </c>
-      <c r="R2" t="s">
-        <v>324</v>
-      </c>
-      <c r="S2" s="33" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -3310,58 +3297,58 @@
         <v>46</v>
       </c>
       <c r="B3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E3" t="s">
+        <v>325</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H3" t="s">
         <v>326</v>
       </c>
-      <c r="C3" t="s">
+      <c r="I3" t="s">
+        <v>312</v>
+      </c>
+      <c r="J3" t="s">
         <v>327</v>
       </c>
-      <c r="D3" t="s">
-        <v>310</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="K3" t="s">
         <v>328</v>
       </c>
-      <c r="F3" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="G3" t="s">
-        <v>313</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>329</v>
       </c>
-      <c r="I3" t="s">
-        <v>315</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
+        <v>316</v>
+      </c>
+      <c r="N3" t="s">
+        <v>317</v>
+      </c>
+      <c r="O3" t="s">
+        <v>318</v>
+      </c>
+      <c r="P3" t="s">
         <v>330</v>
       </c>
-      <c r="K3" t="s">
-        <v>331</v>
-      </c>
-      <c r="L3" t="s">
-        <v>332</v>
-      </c>
-      <c r="M3" t="s">
-        <v>319</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>320</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>321</v>
       </c>
-      <c r="P3" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>323</v>
-      </c>
-      <c r="R3" t="s">
-        <v>324</v>
-      </c>
       <c r="S3" s="33" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3386,13 +3373,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>28</v>
@@ -3403,10 +3390,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>29</v>
@@ -3417,10 +3404,10 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>30</v>
@@ -3452,25 +3439,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>32</v>
@@ -3478,10 +3465,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -3495,24 +3482,24 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" t="s">
+        <v>337</v>
+      </c>
+      <c r="G3" t="s">
         <v>339</v>
-      </c>
-      <c r="B3" t="s">
-        <v>340</v>
-      </c>
-      <c r="G3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G4" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3550,10 +3537,10 @@
         <v>34</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>35</v>
@@ -3565,13 +3552,13 @@
         <v>36</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>37</v>
@@ -3583,7 +3570,7 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>38</v>
@@ -3593,7 +3580,7 @@
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>39</v>
@@ -3605,7 +3592,7 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>40</v>
@@ -3615,7 +3602,7 @@
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>41</v>
@@ -3623,11 +3610,11 @@
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>40</v>
@@ -3637,7 +3624,7 @@
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
@@ -3646,11 +3633,11 @@
     </row>
     <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>40</v>
@@ -3660,7 +3647,7 @@
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
@@ -3926,16 +3913,16 @@
         <v>59</v>
       </c>
       <c r="B2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
         <v>264</v>
       </c>
-      <c r="C2" t="s">
-        <v>268</v>
-      </c>
-      <c r="D2" t="s">
-        <v>266</v>
-      </c>
       <c r="E2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F2" t="s">
         <v>44</v>
@@ -3944,24 +3931,24 @@
         <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
         <v>46</v>
@@ -3970,7 +3957,7 @@
         <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3996,87 +3983,87 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4108,144 +4095,144 @@
         <v>42</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -4275,101 +4262,101 @@
         <v>42</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D3" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="28" t="s">
         <v>240</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D4" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>240</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="D6" s="28" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -4421,39 +4408,39 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="D3" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="D3" t="s">
-        <v>239</v>
-      </c>
       <c r="E3" s="26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -4476,18 +4463,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4512,10 +4499,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="36"/>
@@ -4523,10 +4510,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -4546,7 +4533,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
@@ -4557,7 +4544,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
@@ -4568,7 +4555,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
@@ -4579,7 +4566,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
@@ -4590,7 +4577,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
@@ -4598,10 +4585,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
@@ -4609,10 +4596,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
@@ -4620,19 +4607,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>152</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>15</v>
@@ -4640,42 +4627,42 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -4727,53 +4714,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>144</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>252</v>
-      </c>
       <c r="C2" s="28" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>253</v>
-      </c>
       <c r="C3" s="28" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4801,13 +4788,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>133</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4815,43 +4802,43 @@
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -4859,10 +4846,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -4891,60 +4878,60 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>
@@ -4952,13 +4939,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -4968,139 +4955,139 @@
         <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>362</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="10" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="10" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>15</v>
@@ -5110,46 +5097,46 @@
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="10" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="L8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="M8" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -5160,15 +5147,15 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
@@ -5187,7 +5174,7 @@
     </row>
     <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="2"/>
@@ -5204,10 +5191,10 @@
     </row>
     <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
@@ -5218,10 +5205,10 @@
     </row>
     <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>1</v>
@@ -5235,7 +5222,7 @@
     </row>
     <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C14"/>
       <c r="D14" s="1" t="s">
@@ -5244,7 +5231,7 @@
     </row>
     <row r="15" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="1" t="s">
@@ -5277,10 +5264,10 @@
     </row>
     <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -5291,10 +5278,10 @@
     </row>
     <row r="17" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -5302,7 +5289,7 @@
     </row>
     <row r="18" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C18"/>
       <c r="G18" s="1" t="s">
@@ -5323,7 +5310,7 @@
     </row>
     <row r="19" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C19"/>
       <c r="D19" s="1" t="s">
@@ -5359,10 +5346,10 @@
     </row>
     <row r="20" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>1</v>
@@ -5373,7 +5360,7 @@
     </row>
     <row r="21" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C21"/>
       <c r="H21" s="1" t="s">
@@ -5385,10 +5372,10 @@
     </row>
     <row r="22" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>1</v>
@@ -5399,10 +5386,10 @@
     </row>
     <row r="23" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>1</v>
@@ -5413,7 +5400,7 @@
     </row>
     <row r="24" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C24"/>
       <c r="D24" s="1" t="s">
@@ -5425,12 +5412,12 @@
     </row>
     <row r="25" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>1</v>
@@ -5438,7 +5425,7 @@
     </row>
     <row r="27" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1</v>
@@ -5449,7 +5436,7 @@
     </row>
     <row r="28" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>1</v>
@@ -5460,7 +5447,7 @@
     </row>
     <row r="29" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>1</v>
@@ -5477,7 +5464,7 @@
     </row>
     <row r="30" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>1</v>
@@ -5485,7 +5472,7 @@
     </row>
     <row r="31" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>1</v>
@@ -5493,7 +5480,7 @@
     </row>
     <row r="32" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>1</v>
@@ -5501,7 +5488,7 @@
     </row>
     <row r="33" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>1</v>
@@ -5509,12 +5496,12 @@
     </row>
     <row r="34" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="20" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
@@ -5522,7 +5509,7 @@
     </row>
     <row r="36" spans="2:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>1</v>
@@ -5533,7 +5520,7 @@
     </row>
     <row r="37" spans="2:16" ht="34" x14ac:dyDescent="0.2">
       <c r="B37" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>1</v>
@@ -5568,39 +5555,39 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E1" t="s">
+        <v>417</v>
+      </c>
+      <c r="F1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G1" t="s">
         <v>419</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>420</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>421</v>
-      </c>
-      <c r="G1" t="s">
-        <v>422</v>
-      </c>
-      <c r="H1" t="s">
-        <v>423</v>
-      </c>
-      <c r="I1" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>
@@ -5614,13 +5601,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -5636,68 +5623,68 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="H4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D5" t="s">
+        <v>417</v>
+      </c>
+      <c r="E5" t="s">
+        <v>418</v>
+      </c>
+      <c r="F5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G5" t="s">
         <v>420</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>421</v>
       </c>
-      <c r="F5" t="s">
-        <v>422</v>
-      </c>
-      <c r="G5" t="s">
-        <v>423</v>
-      </c>
-      <c r="H5" t="s">
-        <v>424</v>
-      </c>
       <c r="I5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="10" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="10" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="10" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5708,15 +5695,15 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -5726,10 +5713,10 @@
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>1</v>
@@ -5741,7 +5728,7 @@
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="30" t="s">
@@ -5756,7 +5743,7 @@
     </row>
     <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="30" t="s">
@@ -5771,10 +5758,10 @@
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>1</v>
@@ -5786,7 +5773,7 @@
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="30" t="s">
@@ -5800,7 +5787,7 @@
     </row>
     <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>1</v>
@@ -5812,7 +5799,7 @@
     </row>
     <row r="17" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>1</v>
@@ -5824,7 +5811,7 @@
     </row>
     <row r="18" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="20" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>1</v>
@@ -5839,7 +5826,7 @@
     </row>
     <row r="19" spans="2:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
@@ -5849,7 +5836,7 @@
     </row>
     <row r="20" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>1</v>
@@ -5862,7 +5849,7 @@
     </row>
     <row r="21" spans="2:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" s="20" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>1</v>
@@ -5902,66 +5889,66 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D1" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G1" t="s">
         <v>390</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>391</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>392</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>393</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>394</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>395</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>396</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>397</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>398</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>399</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>400</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>401</v>
-      </c>
-      <c r="P1" t="s">
-        <v>402</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>403</v>
-      </c>
-      <c r="R1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>
@@ -5983,13 +5970,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -6013,108 +6000,108 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="H4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="L4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="M4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="N4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="O4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="P4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="Q4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="R4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D5" t="s">
+        <v>388</v>
+      </c>
+      <c r="E5" t="s">
+        <v>389</v>
+      </c>
+      <c r="F5" t="s">
+        <v>390</v>
+      </c>
+      <c r="G5" t="s">
         <v>391</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>392</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>393</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>394</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>395</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>396</v>
       </c>
-      <c r="J5" t="s">
+      <c r="M5" t="s">
         <v>397</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>398</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>399</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>400</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>401</v>
       </c>
-      <c r="O5" t="s">
-        <v>402</v>
-      </c>
-      <c r="P5" t="s">
-        <v>403</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>404</v>
-      </c>
       <c r="R5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="10" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D6" s="23"/>
     </row>
@@ -6122,7 +6109,7 @@
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="10" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D7" s="23"/>
     </row>
@@ -6130,7 +6117,7 @@
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="10" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D8" s="23"/>
     </row>
@@ -6142,15 +6129,15 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q10" s="5" t="s">
         <v>1</v>
@@ -6159,7 +6146,7 @@
     </row>
     <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C11"/>
       <c r="E11" s="5" t="s">
@@ -6169,10 +6156,10 @@
     </row>
     <row r="12" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>1</v>
@@ -6196,7 +6183,7 @@
     </row>
     <row r="13" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>1</v>
@@ -6220,7 +6207,7 @@
     </row>
     <row r="14" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>1</v>
@@ -6265,7 +6252,7 @@
     </row>
     <row r="15" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>1</v>
@@ -6310,7 +6297,7 @@
     </row>
     <row r="16" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -6338,7 +6325,7 @@
     </row>
     <row r="17" spans="2:18" ht="34" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -6368,10 +6355,10 @@
     </row>
     <row r="18" spans="2:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R18" t="s">
         <v>1</v>
@@ -6403,834 +6390,834 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D1" s="35" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="35" t="s">
+        <v>360</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>361</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>364</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>365</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>366</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G2" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F3" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G3" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="H3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G4" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G5" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H5" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E6" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F6" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G6" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G7" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E8" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G8" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" t="s">
         <v>379</v>
-      </c>
-      <c r="B9" t="s">
-        <v>382</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E9" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F9" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G9" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H9" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B10" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E10" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F10" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G10" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E11" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F11" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G11" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H11" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B12" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E12" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F12" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G12" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="H12" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E13" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F13" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G13" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H13" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>383</v>
+      </c>
+      <c r="B14" t="s">
         <v>386</v>
-      </c>
-      <c r="B14" t="s">
-        <v>389</v>
       </c>
       <c r="C14"/>
       <c r="D14" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E14" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F14" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G14" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H14" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B15" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E15" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F15" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G15" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H15" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E16" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F16" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G16" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B17" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E17" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F17" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G17" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H17" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B18" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E18" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F18" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G18" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H18" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B19" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C19"/>
       <c r="D19" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E19" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F19" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G19" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H19" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B20" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C20"/>
       <c r="D20" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E20" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G20" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H20" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B21" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C21"/>
       <c r="D21" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E21" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F21" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G21" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H21" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B22" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C22"/>
       <c r="D22" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E22" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F22" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G22" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="H22" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B23" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C23"/>
       <c r="D23" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E23" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F23" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G23" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H23" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B24" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C24"/>
       <c r="D24" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E24" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="F24" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G24" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H24" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B25" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E25" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="F25" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G25" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H25" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B26" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C26"/>
       <c r="D26" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E26" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F26" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G26" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H26" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B27" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C27"/>
       <c r="D27" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E27" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="F27" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G27" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="H27" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B28" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C28"/>
       <c r="D28" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E28" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F28" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G28" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H28" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E29" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F29" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H29" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B30" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C30"/>
       <c r="D30" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E30" t="s">
+        <v>416</v>
+      </c>
+      <c r="F30" t="s">
         <v>419</v>
       </c>
-      <c r="F30" t="s">
-        <v>422</v>
-      </c>
       <c r="G30" s="23" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H30" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B31" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C31"/>
       <c r="D31" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E31" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F31" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G31" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H31" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B32" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C32"/>
       <c r="D32" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E32" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F32" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G32" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H32" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E33" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F33" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G33" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H33"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B34" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C34"/>
       <c r="D34" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E34" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F34" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G34" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H34" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E35" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F35" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G35" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H35" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>